<commit_message>
[MS-DWSS]: Fix watchman warnings.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-DWSS/MS-DWSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-DWSS/MS-DWSS_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15450" windowHeight="10560" tabRatio="570"/>
@@ -5822,10 +5822,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-DWSS_R261, MS-DWSS_R262 and MS-DWSS_R263.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In GetDwsMetaDataResponse] If the site is not one of those types ["DWS", "MWS", or an empty string.], an empty string MUST be returned.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5982,9 +5978,6 @@
     <t>[In Appendix B: Product Behavior] Implementation does return the Schema element for Tasks. (Windows SharePoint Services 3.0, SharePoint Foundation 2010, and Microsoft SharePoint Server 2016 and above follow this behavior.)</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-DWSS_R256, MS-DWSS_R257 and MS-DWSS_R258.</t>
-  </si>
-  <si>
     <t>Verified by derived requirements: MS-DWSS_R2561, MS-DWSS_R2562.</t>
   </si>
   <si>
@@ -6007,6 +6000,12 @@
   </si>
   <si>
     <t>Verified by derived requirement: MS-DWSS_R1682.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-DWSS_R256, MS-DWSS_R257, MS-DWSS_R258.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-DWSS_R261, MS-DWSS_R262, MS-DWSS_R263.</t>
   </si>
 </sst>
 </file>
@@ -6394,6 +6393,21 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6417,21 +6431,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10910,7 +10909,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>1464</v>
@@ -10921,127 +10920,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -11054,12 +11053,12 @@
       <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -11072,12 +11071,12 @@
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -11090,12 +11089,12 @@
       <c r="C14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -11108,60 +11107,60 @@
       <c r="C15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="81" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="73" t="s">
         <v>1461</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -22321,10 +22320,10 @@
         <v>6</v>
       </c>
       <c r="G462" s="43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H462" s="42" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I462" s="45"/>
     </row>
@@ -24306,7 +24305,7 @@
         <v>17</v>
       </c>
       <c r="I540" s="45" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="541" spans="1:9" customFormat="1" ht="30">
@@ -24635,7 +24634,7 @@
         <v>17</v>
       </c>
       <c r="I553" s="45" t="s">
-        <v>1581</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="554" spans="1:9" customFormat="1" ht="45">
@@ -24646,7 +24645,7 @@
         <v>1067</v>
       </c>
       <c r="C554" s="30" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="D554" s="26"/>
       <c r="E554" s="28" t="s">
@@ -24662,7 +24661,7 @@
         <v>17</v>
       </c>
       <c r="I554" s="45" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="555" spans="1:9" customFormat="1">
@@ -24673,7 +24672,7 @@
         <v>1067</v>
       </c>
       <c r="C555" s="27" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="D555" s="26"/>
       <c r="E555" s="28" t="s">
@@ -24698,7 +24697,7 @@
         <v>1067</v>
       </c>
       <c r="C556" s="30" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="D556" s="26"/>
       <c r="E556" s="28" t="s">
@@ -24764,7 +24763,7 @@
         <v>17</v>
       </c>
       <c r="I558" s="45" t="s">
-        <v>1541</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="559" spans="1:9" customFormat="1">
@@ -24775,7 +24774,7 @@
         <v>1067</v>
       </c>
       <c r="C559" s="27" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="D559" s="26"/>
       <c r="E559" s="28" t="s">
@@ -24800,7 +24799,7 @@
         <v>1067</v>
       </c>
       <c r="C560" s="27" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="D560" s="26"/>
       <c r="E560" s="28" t="s">
@@ -24825,7 +24824,7 @@
         <v>1067</v>
       </c>
       <c r="C561" s="27" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="D561" s="26"/>
       <c r="E561" s="28" t="s">
@@ -25125,7 +25124,7 @@
         <v>1067</v>
       </c>
       <c r="C573" s="30" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="D573" s="26"/>
       <c r="E573" s="28" t="s">
@@ -25150,7 +25149,7 @@
         <v>1067</v>
       </c>
       <c r="C574" s="30" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="D574" s="26"/>
       <c r="E574" s="28" t="s">
@@ -25175,7 +25174,7 @@
         <v>1067</v>
       </c>
       <c r="C575" s="30" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="D575" s="26"/>
       <c r="E575" s="28" t="s">
@@ -25304,7 +25303,7 @@
         <v>1067</v>
       </c>
       <c r="C580" s="27" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="D580" s="26"/>
       <c r="E580" s="28" t="s">
@@ -25354,7 +25353,7 @@
         <v>1143</v>
       </c>
       <c r="C582" s="27" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="D582" s="26"/>
       <c r="E582" s="28" t="s">
@@ -25379,7 +25378,7 @@
         <v>1143</v>
       </c>
       <c r="C583" s="30" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="D583" s="26"/>
       <c r="E583" s="28" t="s">
@@ -25454,7 +25453,7 @@
         <v>1143</v>
       </c>
       <c r="C586" s="27" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D586" s="26"/>
       <c r="E586" s="28" t="s">
@@ -25470,7 +25469,7 @@
         <v>17</v>
       </c>
       <c r="I586" s="51" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="587" spans="1:9" customFormat="1">
@@ -25481,7 +25480,7 @@
         <v>1143</v>
       </c>
       <c r="C587" s="30" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="D587" s="26"/>
       <c r="E587" s="28" t="s">
@@ -25556,7 +25555,7 @@
         <v>1143</v>
       </c>
       <c r="C590" s="27" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="D590" s="26"/>
       <c r="E590" s="28" t="s">
@@ -27082,7 +27081,7 @@
         <v>1283</v>
       </c>
       <c r="C651" s="30" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="D651" s="26"/>
       <c r="E651" s="28" t="s">
@@ -27532,7 +27531,7 @@
         <v>1319</v>
       </c>
       <c r="C669" s="30" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="D669" s="26"/>
       <c r="E669" s="28" t="s">
@@ -27557,7 +27556,7 @@
         <v>1319</v>
       </c>
       <c r="C670" s="30" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="D670" s="26"/>
       <c r="E670" s="28" t="s">
@@ -27839,7 +27838,7 @@
         <v>1370</v>
       </c>
       <c r="D681" s="41" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="E681" s="42" t="s">
         <v>22</v>
@@ -28013,7 +28012,7 @@
         <v>1379</v>
       </c>
       <c r="D687" s="41" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="E687" s="28" t="s">
         <v>22</v>
@@ -28040,7 +28039,7 @@
         <v>1375</v>
       </c>
       <c r="D688" s="41" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="E688" s="28" t="s">
         <v>22</v>
@@ -28067,7 +28066,7 @@
         <v>1374</v>
       </c>
       <c r="D689" s="41" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="E689" s="28" t="s">
         <v>22</v>
@@ -28091,10 +28090,10 @@
         <v>1339</v>
       </c>
       <c r="C690" s="45" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="D690" s="41" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="E690" s="42" t="s">
         <v>22</v>
@@ -28120,7 +28119,7 @@
         <v>1345</v>
       </c>
       <c r="C691" s="45" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D691" s="41"/>
       <c r="E691" s="28" t="s">
@@ -28145,7 +28144,7 @@
         <v>1339</v>
       </c>
       <c r="C692" s="47" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="D692" s="36" t="s">
         <v>1376</v>
@@ -28174,7 +28173,7 @@
         <v>1339</v>
       </c>
       <c r="C693" s="48" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="D693" s="36" t="s">
         <v>1376</v>
@@ -28203,7 +28202,7 @@
         <v>1339</v>
       </c>
       <c r="C694" s="48" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D694" s="36" t="s">
         <v>1376</v>
@@ -28232,10 +28231,10 @@
         <v>1345</v>
       </c>
       <c r="C695" s="45" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="D695" s="36" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="E695" s="28" t="s">
         <v>22</v>
@@ -28255,16 +28254,16 @@
     </row>
     <row r="696" spans="1:9" s="39" customFormat="1" ht="30">
       <c r="A696" s="59" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B696" s="36" t="s">
         <v>1339</v>
       </c>
       <c r="C696" s="45" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="D696" s="36" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="E696" s="42" t="s">
         <v>22</v>
@@ -28288,10 +28287,10 @@
         <v>1339</v>
       </c>
       <c r="C697" s="45" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="D697" s="36" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="E697" s="42" t="s">
         <v>22</v>
@@ -28311,16 +28310,16 @@
     </row>
     <row r="698" spans="1:9" s="39" customFormat="1" ht="45">
       <c r="A698" s="61" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="B698" s="36" t="s">
         <v>1339</v>
       </c>
       <c r="C698" s="54" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D698" s="36" t="s">
         <v>1561</v>
-      </c>
-      <c r="D698" s="36" t="s">
-        <v>1562</v>
       </c>
       <c r="E698" s="42" t="s">
         <v>22</v>
@@ -28338,16 +28337,16 @@
     </row>
     <row r="699" spans="1:9" s="39" customFormat="1" ht="45">
       <c r="A699" s="61" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="B699" s="36" t="s">
         <v>1339</v>
       </c>
       <c r="C699" s="54" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D699" s="36" t="s">
         <v>1576</v>
-      </c>
-      <c r="D699" s="36" t="s">
-        <v>1577</v>
       </c>
       <c r="E699" s="42" t="s">
         <v>22</v>
@@ -28367,16 +28366,16 @@
     </row>
     <row r="700" spans="1:9" s="39" customFormat="1" ht="45">
       <c r="A700" s="61" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B700" s="36" t="s">
         <v>1339</v>
       </c>
       <c r="C700" s="54" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="D700" s="36" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="E700" s="42" t="s">
         <v>22</v>
@@ -28396,13 +28395,13 @@
     </row>
     <row r="701" spans="1:9" customFormat="1">
       <c r="A701" s="25" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B701" s="26" t="s">
         <v>1345</v>
       </c>
       <c r="C701" s="45" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D701" s="26"/>
       <c r="E701" s="28" t="s">
@@ -28425,11 +28424,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -28437,6 +28431,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A577:B577 I619:I622 I678:I679 A293:B293 A513:C513 A116:C128 A131:C141 A516:C521 D524 A115:G115 A227:D227 A689:B690 I199 A687:C688 A691:C691 A239:C292 I41:I63 A309:I341 B168:D169 I168:I169 D294:H294 D116:H141 D576:D577 D523:E523 A143:I149 A343:I352 A151:I154 A150:H150 A156:I157 A155:H155 A159:I161 A158:H158 A228:H238 A525:D525 A528:D528 A142:H142 A342:H342 E655:I662 E654:H654 E664:I672 E663:H663 E674:I675 E673:H673 E676:H679 D516:H522 A514:D515 A195:H195 A353:H353 D239:I293 A20:H114 A163:I163 A162:H162 E623:I653 A295:I307 A308:H308 A354:I460 A578:D679 A701:D701 A170:I193 A692:D694 A684:D684 A681:I683 A680:H680 B164:I164 E165:H169 A197:H226 A463:I486 I496:I514 A487:D512 E487:H514 I538:I544 A531:D575 E525:H622 A695:C700 E684:H701 I546:I561">
@@ -30930,12 +30929,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -30984,6 +30977,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -30994,20 +30993,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31022,6 +31007,20 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update code for MS-DWSS
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-DWSS/MS-DWSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-DWSS/MS-DWSS_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D86CE3-7FC9-482C-9CFD-01B488614575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FF6C67-E60E-4A6A-A32A-9902BDAE08CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21105" windowHeight="12480" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -4153,9 +4153,6 @@
   </si>
   <si>
     <t>MS-DWSS_R628</t>
-  </si>
-  <si>
-    <t>[In ListInfo] The following elements MUST be present if, and only if, the user has that permission: InsertListIems, EditListItems, DeleteListItems, and ManageLists.</t>
   </si>
   <si>
     <t>MS-DWSS_R629</t>
@@ -5990,6 +5987,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>[In Appendix B: Product Behavior] Implementation does return HTTP status code 401 with response body which contains text "401 Unauthorized" instead of the "NoAccess" error if the authenticated user is not permitted to access this information. (Windows SharePoint Services 3.0, SharePoint Foundation 2010, SharePoint Foundation 2013, and SharePoint Server 2016 will never return the "NoAccess" error code; instead, these product versions will return HTTP status code 401 with a response body containing the text "401 Unauthorized".)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>MS-DWSS_R4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6010,10 +6011,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] Implementation does return HTTP status code 401 with response body which contains text "401 Unauthorized" instead of the "NoAccess" error if the authenticated user is not permitted to access this information. (Windows SharePoint Services 3.0, SharePoint Foundation 2010, SharePoint Foundation 2013, SharePoint Server 2016 and SharePoint Server 2019 will never return the "NoAccess" error code; instead, these product versions will return HTTP status code 401 with a response body containing the text "401 Unauthorized".)</t>
-  </si>
-  <si>
-    <t>12.0</t>
+    <t>[In ListInfo] The following elements MUST be present if, and only if, the user has that permission: InsertListItems, EditListItems, DeleteListItems, and ManageLists.</t>
+  </si>
+  <si>
+    <t>14.0</t>
   </si>
 </sst>
 </file>
@@ -6402,21 +6403,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6440,6 +6426,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10876,12 +10877,12 @@
   <dimension ref="A1:L702"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="11" customWidth="1"/>
     <col min="2" max="2" width="6" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
@@ -10896,7 +10897,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -10906,7 +10907,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -10923,135 +10924,135 @@
         <v>1589</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="F3" s="13">
-        <v>44308</v>
+        <v>44397</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="30">
+    <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -11064,12 +11065,12 @@
       <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -11082,12 +11083,12 @@
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -11100,12 +11101,12 @@
       <c r="C14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -11118,60 +11119,60 @@
       <c r="C15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="81" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="73" t="s">
-        <v>1455</v>
-      </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
+      <c r="B17" s="68" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -11213,7 +11214,7 @@
         <v>43</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="28" t="s">
@@ -11238,7 +11239,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="28" t="s">
@@ -11288,7 +11289,7 @@
         <v>43</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="28" t="s">
@@ -11313,7 +11314,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="28" t="s">
@@ -11363,7 +11364,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="28" t="s">
@@ -11454,7 +11455,7 @@
         <v>17</v>
       </c>
       <c r="I29" s="45" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="30" spans="1:12" customFormat="1" ht="30">
@@ -11465,7 +11466,7 @@
         <v>56</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D30" s="26"/>
       <c r="E30" s="28" t="s">
@@ -11490,7 +11491,7 @@
         <v>56</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="28" t="s">
@@ -11515,7 +11516,7 @@
         <v>63</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="28" t="s">
@@ -11815,7 +11816,7 @@
         <v>85</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="D44" s="26"/>
       <c r="E44" s="28" t="s">
@@ -11916,7 +11917,7 @@
         <v>85</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="D48" s="26"/>
       <c r="E48" s="28" t="s">
@@ -11966,7 +11967,7 @@
         <v>100</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="D50" s="26"/>
       <c r="E50" s="28" t="s">
@@ -12066,7 +12067,7 @@
         <v>108</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="28" t="s">
@@ -12216,7 +12217,7 @@
         <v>110</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="D60" s="26"/>
       <c r="E60" s="28" t="s">
@@ -13112,7 +13113,7 @@
         <v>192</v>
       </c>
       <c r="C95" s="27" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="D95" s="26"/>
       <c r="E95" s="28" t="s">
@@ -13137,7 +13138,7 @@
         <v>192</v>
       </c>
       <c r="C96" s="30" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="D96" s="26"/>
       <c r="E96" s="28" t="s">
@@ -13237,7 +13238,7 @@
         <v>192</v>
       </c>
       <c r="C100" s="27" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="D100" s="26"/>
       <c r="E100" s="28" t="s">
@@ -13313,7 +13314,7 @@
         <v>192</v>
       </c>
       <c r="C103" s="27" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="D103" s="26"/>
       <c r="E103" s="28" t="s">
@@ -13588,7 +13589,7 @@
         <v>192</v>
       </c>
       <c r="C114" s="27" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="D114" s="26"/>
       <c r="E114" s="28" t="s">
@@ -13604,7 +13605,7 @@
         <v>17</v>
       </c>
       <c r="I114" s="51" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="115" spans="1:9" customFormat="1" ht="30">
@@ -13715,7 +13716,7 @@
         <v>236</v>
       </c>
       <c r="C119" s="27" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="D119" s="26"/>
       <c r="E119" s="28" t="s">
@@ -13790,7 +13791,7 @@
         <v>236</v>
       </c>
       <c r="C122" s="27" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="D122" s="26"/>
       <c r="E122" s="28" t="s">
@@ -13940,7 +13941,7 @@
         <v>236</v>
       </c>
       <c r="C128" s="27" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="D128" s="26"/>
       <c r="E128" s="28" t="s">
@@ -14315,7 +14316,7 @@
         <v>279</v>
       </c>
       <c r="C143" s="30" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="D143" s="26"/>
       <c r="E143" s="28" t="s">
@@ -14340,7 +14341,7 @@
         <v>31</v>
       </c>
       <c r="C144" s="27" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="D144" s="26"/>
       <c r="E144" s="28" t="s">
@@ -14796,7 +14797,7 @@
         <v>31</v>
       </c>
       <c r="C162" s="27" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="D162" s="26"/>
       <c r="E162" s="28" t="s">
@@ -14812,7 +14813,7 @@
         <v>17</v>
       </c>
       <c r="I162" s="51" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="163" spans="1:9" customFormat="1" ht="30">
@@ -14842,13 +14843,13 @@
     </row>
     <row r="164" spans="1:9" s="39" customFormat="1" ht="240">
       <c r="A164" s="42" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B164" s="41" t="s">
         <v>1439</v>
       </c>
-      <c r="B164" s="41" t="s">
-        <v>1440</v>
-      </c>
       <c r="C164" s="45" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="D164" s="42"/>
       <c r="E164" s="42" t="s">
@@ -14867,13 +14868,13 @@
     </row>
     <row r="165" spans="1:9" s="39" customFormat="1" ht="30">
       <c r="A165" s="42" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B165" s="41" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C165" s="45" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="D165" s="42"/>
       <c r="E165" s="42" t="s">
@@ -14892,13 +14893,13 @@
     </row>
     <row r="166" spans="1:9" s="39" customFormat="1" ht="30">
       <c r="A166" s="42" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="B166" s="41" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C166" s="45" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="D166" s="42"/>
       <c r="E166" s="42" t="s">
@@ -14917,13 +14918,13 @@
     </row>
     <row r="167" spans="1:9" s="39" customFormat="1" ht="30">
       <c r="A167" s="42" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="B167" s="41" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C167" s="45" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="D167" s="42"/>
       <c r="E167" s="42" t="s">
@@ -14942,13 +14943,13 @@
     </row>
     <row r="168" spans="1:9" s="39" customFormat="1" ht="30">
       <c r="A168" s="42" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B168" s="53" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C168" s="54" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="D168" s="53"/>
       <c r="E168" s="42" t="s">
@@ -14967,13 +14968,13 @@
     </row>
     <row r="169" spans="1:9" s="39" customFormat="1" ht="30">
       <c r="A169" s="42" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B169" s="53" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C169" s="54" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="D169" s="53"/>
       <c r="E169" s="42" t="s">
@@ -15048,7 +15049,7 @@
         <v>325</v>
       </c>
       <c r="C172" s="27" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="D172" s="26"/>
       <c r="E172" s="28" t="s">
@@ -15173,7 +15174,7 @@
         <v>338</v>
       </c>
       <c r="C177" s="30" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="D177" s="26"/>
       <c r="E177" s="28" t="s">
@@ -15273,7 +15274,7 @@
         <v>338</v>
       </c>
       <c r="C181" s="27" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="D181" s="26"/>
       <c r="E181" s="28" t="s">
@@ -15323,7 +15324,7 @@
         <v>338</v>
       </c>
       <c r="C183" s="27" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="D183" s="26"/>
       <c r="E183" s="28" t="s">
@@ -15348,7 +15349,7 @@
         <v>338</v>
       </c>
       <c r="C184" s="27" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="D184" s="26"/>
       <c r="E184" s="28" t="s">
@@ -15619,13 +15620,13 @@
     </row>
     <row r="195" spans="1:9" customFormat="1" ht="30">
       <c r="A195" s="25" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B195" s="26" t="s">
         <v>338</v>
       </c>
       <c r="C195" s="27" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="D195" s="26"/>
       <c r="E195" s="28" t="s">
@@ -15644,13 +15645,13 @@
     </row>
     <row r="196" spans="1:9" s="39" customFormat="1" ht="30">
       <c r="A196" s="40" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B196" s="41" t="s">
         <v>338</v>
       </c>
       <c r="C196" s="27" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="D196" s="41"/>
       <c r="E196" s="42" t="s">
@@ -15750,7 +15751,7 @@
         <v>382</v>
       </c>
       <c r="C200" s="27" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="D200" s="26"/>
       <c r="E200" s="28" t="s">
@@ -15800,7 +15801,7 @@
         <v>382</v>
       </c>
       <c r="C202" s="27" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="D202" s="26"/>
       <c r="E202" s="28" t="s">
@@ -15825,7 +15826,7 @@
         <v>382</v>
       </c>
       <c r="C203" s="27" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="D203" s="26"/>
       <c r="E203" s="28" t="s">
@@ -15975,7 +15976,7 @@
         <v>392</v>
       </c>
       <c r="C209" s="27" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="D209" s="26"/>
       <c r="E209" s="28" t="s">
@@ -16025,7 +16026,7 @@
         <v>392</v>
       </c>
       <c r="C211" s="27" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="D211" s="26"/>
       <c r="E211" s="28" t="s">
@@ -16125,7 +16126,7 @@
         <v>408</v>
       </c>
       <c r="C215" s="27" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="D215" s="26"/>
       <c r="E215" s="28" t="s">
@@ -16325,7 +16326,7 @@
         <v>408</v>
       </c>
       <c r="C223" s="27" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="D223" s="26"/>
       <c r="E223" s="28" t="s">
@@ -16501,7 +16502,7 @@
         <v>32</v>
       </c>
       <c r="C230" s="30" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="D230" s="26"/>
       <c r="E230" s="28" t="s">
@@ -16876,7 +16877,7 @@
         <v>469</v>
       </c>
       <c r="C245" s="27" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="D245" s="26"/>
       <c r="E245" s="28" t="s">
@@ -16901,7 +16902,7 @@
         <v>469</v>
       </c>
       <c r="C246" s="27" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="D246" s="26"/>
       <c r="E246" s="28" t="s">
@@ -16926,7 +16927,7 @@
         <v>469</v>
       </c>
       <c r="C247" s="27" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="D247" s="26"/>
       <c r="E247" s="28" t="s">
@@ -16951,7 +16952,7 @@
         <v>469</v>
       </c>
       <c r="C248" s="27" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="D248" s="26"/>
       <c r="E248" s="28" t="s">
@@ -16992,7 +16993,7 @@
         <v>17</v>
       </c>
       <c r="I249" s="45" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="250" spans="1:9" customFormat="1" ht="30">
@@ -17428,7 +17429,7 @@
         <v>516</v>
       </c>
       <c r="C267" s="30" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="D267" s="26"/>
       <c r="E267" s="28" t="s">
@@ -17678,7 +17679,7 @@
         <v>538</v>
       </c>
       <c r="C277" s="30" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="D277" s="26"/>
       <c r="E277" s="28" t="s">
@@ -17828,7 +17829,7 @@
         <v>547</v>
       </c>
       <c r="C283" s="27" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="D283" s="26"/>
       <c r="E283" s="28" t="s">
@@ -17928,7 +17929,7 @@
         <v>547</v>
       </c>
       <c r="C287" s="30" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="D287" s="26"/>
       <c r="E287" s="28" t="s">
@@ -18094,7 +18095,7 @@
         <v>17</v>
       </c>
       <c r="I293" s="45" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="294" spans="1:9" customFormat="1" ht="45">
@@ -18157,7 +18158,7 @@
         <v>547</v>
       </c>
       <c r="C296" s="27" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="D296" s="26"/>
       <c r="E296" s="28" t="s">
@@ -18207,7 +18208,7 @@
         <v>547</v>
       </c>
       <c r="C298" s="30" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="D298" s="26"/>
       <c r="E298" s="28" t="s">
@@ -18257,7 +18258,7 @@
         <v>547</v>
       </c>
       <c r="C300" s="27" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="D300" s="26"/>
       <c r="E300" s="28" t="s">
@@ -18357,7 +18358,7 @@
         <v>586</v>
       </c>
       <c r="C304" s="37" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="D304" s="26"/>
       <c r="E304" s="28" t="s">
@@ -18482,7 +18483,7 @@
         <v>602</v>
       </c>
       <c r="C309" s="44" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="D309" s="26"/>
       <c r="E309" s="28" t="s">
@@ -18498,7 +18499,7 @@
         <v>17</v>
       </c>
       <c r="I309" s="45" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="310" spans="1:10" customFormat="1" ht="30">
@@ -18559,7 +18560,7 @@
         <v>586</v>
       </c>
       <c r="C312" s="27" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="D312" s="26"/>
       <c r="E312" s="28" t="s">
@@ -18635,7 +18636,7 @@
         <v>586</v>
       </c>
       <c r="C315" s="27" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D315" s="26"/>
       <c r="E315" s="28" t="s">
@@ -18960,7 +18961,7 @@
         <v>640</v>
       </c>
       <c r="C328" s="30" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="D328" s="26"/>
       <c r="E328" s="28" t="s">
@@ -18985,7 +18986,7 @@
         <v>640</v>
       </c>
       <c r="C329" s="30" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="D329" s="26"/>
       <c r="E329" s="28" t="s">
@@ -19010,7 +19011,7 @@
         <v>640</v>
       </c>
       <c r="C330" s="30" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="D330" s="26"/>
       <c r="E330" s="28" t="s">
@@ -19185,7 +19186,7 @@
         <v>659</v>
       </c>
       <c r="C337" s="30" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="D337" s="26"/>
       <c r="E337" s="28" t="s">
@@ -19210,7 +19211,7 @@
         <v>659</v>
       </c>
       <c r="C338" s="30" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="D338" s="26"/>
       <c r="E338" s="28" t="s">
@@ -19235,7 +19236,7 @@
         <v>659</v>
       </c>
       <c r="C339" s="30" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="D339" s="26"/>
       <c r="E339" s="28" t="s">
@@ -19310,7 +19311,7 @@
         <v>666</v>
       </c>
       <c r="C342" s="27" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="D342" s="26"/>
       <c r="E342" s="28" t="s">
@@ -19335,7 +19336,7 @@
         <v>670</v>
       </c>
       <c r="C343" s="30" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="D343" s="26"/>
       <c r="E343" s="28" t="s">
@@ -19410,7 +19411,7 @@
         <v>676</v>
       </c>
       <c r="C346" s="30" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="D346" s="26"/>
       <c r="E346" s="28" t="s">
@@ -19486,7 +19487,7 @@
         <v>682</v>
       </c>
       <c r="C349" s="30" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="D349" s="26"/>
       <c r="E349" s="28" t="s">
@@ -19586,7 +19587,7 @@
         <v>682</v>
       </c>
       <c r="C353" s="30" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="D353" s="26"/>
       <c r="E353" s="28" t="s">
@@ -19602,7 +19603,7 @@
         <v>17</v>
       </c>
       <c r="I353" s="45" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="354" spans="1:9" customFormat="1" ht="30">
@@ -19663,7 +19664,7 @@
         <v>696</v>
       </c>
       <c r="C356" s="30" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="D356" s="26"/>
       <c r="E356" s="28" t="s">
@@ -19688,7 +19689,7 @@
         <v>696</v>
       </c>
       <c r="C357" s="30" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="D357" s="26"/>
       <c r="E357" s="28" t="s">
@@ -19713,7 +19714,7 @@
         <v>696</v>
       </c>
       <c r="C358" s="30" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="D358" s="26"/>
       <c r="E358" s="28" t="s">
@@ -19888,7 +19889,7 @@
         <v>715</v>
       </c>
       <c r="C365" s="30" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="D365" s="26"/>
       <c r="E365" s="28" t="s">
@@ -19913,7 +19914,7 @@
         <v>715</v>
       </c>
       <c r="C366" s="30" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="D366" s="26"/>
       <c r="E366" s="28" t="s">
@@ -19938,7 +19939,7 @@
         <v>715</v>
       </c>
       <c r="C367" s="30" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="D367" s="26"/>
       <c r="E367" s="28" t="s">
@@ -20188,7 +20189,7 @@
         <v>741</v>
       </c>
       <c r="C377" s="30" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="D377" s="26"/>
       <c r="E377" s="28" t="s">
@@ -20338,7 +20339,7 @@
         <v>741</v>
       </c>
       <c r="C383" s="27" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="D383" s="26"/>
       <c r="E383" s="28" t="s">
@@ -20363,7 +20364,7 @@
         <v>754</v>
       </c>
       <c r="C384" s="30" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D384" s="26"/>
       <c r="E384" s="28" t="s">
@@ -20388,7 +20389,7 @@
         <v>754</v>
       </c>
       <c r="C385" s="30" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D385" s="26"/>
       <c r="E385" s="28" t="s">
@@ -20413,7 +20414,7 @@
         <v>754</v>
       </c>
       <c r="C386" s="30" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="D386" s="26"/>
       <c r="E386" s="28" t="s">
@@ -20588,7 +20589,7 @@
         <v>773</v>
       </c>
       <c r="C393" s="30" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="D393" s="26"/>
       <c r="E393" s="28" t="s">
@@ -20613,7 +20614,7 @@
         <v>773</v>
       </c>
       <c r="C394" s="30" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="D394" s="26"/>
       <c r="E394" s="28" t="s">
@@ -20638,7 +20639,7 @@
         <v>773</v>
       </c>
       <c r="C395" s="30" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="D395" s="26"/>
       <c r="E395" s="28" t="s">
@@ -21004,7 +21005,7 @@
         <v>17</v>
       </c>
       <c r="I409" s="45" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="410" spans="1:9" customFormat="1" ht="45">
@@ -21015,7 +21016,7 @@
         <v>812</v>
       </c>
       <c r="C410" s="30" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="D410" s="26"/>
       <c r="E410" s="28" t="s">
@@ -21040,7 +21041,7 @@
         <v>812</v>
       </c>
       <c r="C411" s="30" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="D411" s="26"/>
       <c r="E411" s="28" t="s">
@@ -21065,7 +21066,7 @@
         <v>812</v>
       </c>
       <c r="C412" s="30" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="D412" s="26"/>
       <c r="E412" s="28" t="s">
@@ -21240,7 +21241,7 @@
         <v>831</v>
       </c>
       <c r="C419" s="30" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="D419" s="26"/>
       <c r="E419" s="28" t="s">
@@ -21265,7 +21266,7 @@
         <v>831</v>
       </c>
       <c r="C420" s="30" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="D420" s="26"/>
       <c r="E420" s="28" t="s">
@@ -21290,7 +21291,7 @@
         <v>831</v>
       </c>
       <c r="C421" s="30" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="D421" s="26"/>
       <c r="E421" s="28" t="s">
@@ -21365,7 +21366,7 @@
         <v>838</v>
       </c>
       <c r="C424" s="27" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="D424" s="26"/>
       <c r="E424" s="28" t="s">
@@ -21515,7 +21516,7 @@
         <v>853</v>
       </c>
       <c r="C430" s="30" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D430" s="26"/>
       <c r="E430" s="28" t="s">
@@ -21581,7 +21582,7 @@
         <v>17</v>
       </c>
       <c r="I432" s="45" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="433" spans="1:9" customFormat="1" ht="30">
@@ -21692,7 +21693,7 @@
         <v>867</v>
       </c>
       <c r="C437" s="30" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="D437" s="26"/>
       <c r="E437" s="28" t="s">
@@ -21717,7 +21718,7 @@
         <v>867</v>
       </c>
       <c r="C438" s="30" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="D438" s="26"/>
       <c r="E438" s="28" t="s">
@@ -21892,7 +21893,7 @@
         <v>887</v>
       </c>
       <c r="C445" s="30" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="D445" s="26"/>
       <c r="E445" s="28" t="s">
@@ -21917,7 +21918,7 @@
         <v>887</v>
       </c>
       <c r="C446" s="30" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="D446" s="26"/>
       <c r="E446" s="28" t="s">
@@ -21942,7 +21943,7 @@
         <v>887</v>
       </c>
       <c r="C447" s="30" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D447" s="26"/>
       <c r="E447" s="28" t="s">
@@ -22017,7 +22018,7 @@
         <v>894</v>
       </c>
       <c r="C450" s="27" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="D450" s="26"/>
       <c r="E450" s="28" t="s">
@@ -22042,7 +22043,7 @@
         <v>894</v>
       </c>
       <c r="C451" s="27" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="D451" s="26"/>
       <c r="E451" s="28" t="s">
@@ -22133,7 +22134,7 @@
         <v>17</v>
       </c>
       <c r="I454" s="45" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="455" spans="1:9" customFormat="1" ht="30">
@@ -22246,7 +22247,7 @@
         <v>908</v>
       </c>
       <c r="C459" s="30" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="D459" s="26"/>
       <c r="E459" s="28" t="s">
@@ -22290,13 +22291,13 @@
     </row>
     <row r="461" spans="1:9" s="39" customFormat="1" ht="30">
       <c r="A461" s="40" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="B461" s="41" t="s">
         <v>916</v>
       </c>
       <c r="C461" s="44" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="D461" s="41"/>
       <c r="E461" s="42" t="s">
@@ -22315,13 +22316,13 @@
     </row>
     <row r="462" spans="1:9" s="39" customFormat="1" ht="409.5">
       <c r="A462" s="40" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="B462" s="41" t="s">
         <v>916</v>
       </c>
       <c r="C462" s="44" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="D462" s="41"/>
       <c r="E462" s="42" t="s">
@@ -22446,7 +22447,7 @@
         <v>908</v>
       </c>
       <c r="C467" s="27" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="D467" s="26"/>
       <c r="E467" s="28" t="s">
@@ -23121,7 +23122,7 @@
         <v>977</v>
       </c>
       <c r="C494" s="30" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="D494" s="26"/>
       <c r="E494" s="28" t="s">
@@ -23146,7 +23147,7 @@
         <v>977</v>
       </c>
       <c r="C495" s="30" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="D495" s="26"/>
       <c r="E495" s="28" t="s">
@@ -23371,7 +23372,7 @@
         <v>1000</v>
       </c>
       <c r="C504" s="30" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="D504" s="26"/>
       <c r="E504" s="28" t="s">
@@ -23397,7 +23398,7 @@
         <v>1000</v>
       </c>
       <c r="C505" s="30" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="D505" s="26"/>
       <c r="E505" s="28" t="s">
@@ -23472,7 +23473,7 @@
         <v>1005</v>
       </c>
       <c r="C508" s="27" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="D508" s="26"/>
       <c r="E508" s="28" t="s">
@@ -23497,7 +23498,7 @@
         <v>1011</v>
       </c>
       <c r="C509" s="30" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="D509" s="26"/>
       <c r="E509" s="28" t="s">
@@ -23522,7 +23523,7 @@
         <v>1011</v>
       </c>
       <c r="C510" s="30" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="D510" s="26"/>
       <c r="E510" s="28" t="s">
@@ -23572,7 +23573,7 @@
         <v>1005</v>
       </c>
       <c r="C512" s="30" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="D512" s="26"/>
       <c r="E512" s="28" t="s">
@@ -23625,7 +23626,7 @@
         <v>1019</v>
       </c>
       <c r="D514" s="41" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="E514" s="28" t="s">
         <v>19</v>
@@ -23727,7 +23728,7 @@
         <v>1027</v>
       </c>
       <c r="D518" s="26" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="E518" s="28" t="s">
         <v>19</v>
@@ -23754,7 +23755,7 @@
         <v>1029</v>
       </c>
       <c r="D519" s="41" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="E519" s="28" t="s">
         <v>19</v>
@@ -23781,7 +23782,7 @@
         <v>1031</v>
       </c>
       <c r="D520" s="41" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="E520" s="28" t="s">
         <v>19</v>
@@ -23808,7 +23809,7 @@
         <v>1033</v>
       </c>
       <c r="D521" s="26" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E521" s="28" t="s">
         <v>19</v>
@@ -24072,7 +24073,7 @@
         <v>1056</v>
       </c>
       <c r="D531" s="26" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E531" s="28" t="s">
         <v>19</v>
@@ -24099,7 +24100,7 @@
         <v>1058</v>
       </c>
       <c r="D532" s="26" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E532" s="28" t="s">
         <v>19</v>
@@ -24126,7 +24127,7 @@
         <v>1060</v>
       </c>
       <c r="D533" s="26" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E533" s="28" t="s">
         <v>19</v>
@@ -24175,7 +24176,7 @@
         <v>1062</v>
       </c>
       <c r="C535" s="30" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D535" s="26"/>
       <c r="E535" s="28" t="s">
@@ -24200,7 +24201,7 @@
         <v>1062</v>
       </c>
       <c r="C536" s="30" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D536" s="26"/>
       <c r="E536" s="28" t="s">
@@ -24275,7 +24276,7 @@
         <v>1062</v>
       </c>
       <c r="C539" s="27" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="D539" s="26"/>
       <c r="E539" s="28" t="s">
@@ -24300,7 +24301,7 @@
         <v>1062</v>
       </c>
       <c r="C540" s="27" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="D540" s="26"/>
       <c r="E540" s="28" t="s">
@@ -24316,7 +24317,7 @@
         <v>17</v>
       </c>
       <c r="I540" s="45" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="541" spans="1:9" customFormat="1" ht="30">
@@ -24327,7 +24328,7 @@
         <v>1062</v>
       </c>
       <c r="C541" s="27" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="D541" s="26"/>
       <c r="E541" s="28" t="s">
@@ -24402,7 +24403,7 @@
         <v>1062</v>
       </c>
       <c r="C544" s="27" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="D544" s="26"/>
       <c r="E544" s="28" t="s">
@@ -24427,7 +24428,7 @@
         <v>1062</v>
       </c>
       <c r="C545" s="27" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="D545" s="26"/>
       <c r="E545" s="28" t="s">
@@ -24452,7 +24453,7 @@
         <v>1062</v>
       </c>
       <c r="C546" s="30" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="D546" s="26"/>
       <c r="E546" s="28" t="s">
@@ -24468,7 +24469,7 @@
         <v>17</v>
       </c>
       <c r="I546" s="45" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="547" spans="1:9" customFormat="1" ht="30">
@@ -24529,7 +24530,7 @@
         <v>1062</v>
       </c>
       <c r="C549" s="27" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="D549" s="26"/>
       <c r="E549" s="28" t="s">
@@ -24604,7 +24605,7 @@
         <v>1062</v>
       </c>
       <c r="C552" s="27" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="D552" s="26"/>
       <c r="E552" s="28" t="s">
@@ -24629,7 +24630,7 @@
         <v>1062</v>
       </c>
       <c r="C553" s="30" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="D553" s="26"/>
       <c r="E553" s="28" t="s">
@@ -24645,7 +24646,7 @@
         <v>17</v>
       </c>
       <c r="I553" s="45" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="554" spans="1:9" customFormat="1" ht="60">
@@ -24656,7 +24657,7 @@
         <v>1062</v>
       </c>
       <c r="C554" s="30" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="D554" s="26"/>
       <c r="E554" s="28" t="s">
@@ -24672,7 +24673,7 @@
         <v>17</v>
       </c>
       <c r="I554" s="45" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="555" spans="1:9" customFormat="1" ht="30">
@@ -24683,7 +24684,7 @@
         <v>1062</v>
       </c>
       <c r="C555" s="27" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D555" s="26"/>
       <c r="E555" s="28" t="s">
@@ -24708,7 +24709,7 @@
         <v>1062</v>
       </c>
       <c r="C556" s="30" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="D556" s="26"/>
       <c r="E556" s="28" t="s">
@@ -24733,7 +24734,7 @@
         <v>1062</v>
       </c>
       <c r="C557" s="27" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="D557" s="26"/>
       <c r="E557" s="28" t="s">
@@ -24758,7 +24759,7 @@
         <v>1062</v>
       </c>
       <c r="C558" s="27" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="D558" s="26"/>
       <c r="E558" s="28" t="s">
@@ -24774,7 +24775,7 @@
         <v>17</v>
       </c>
       <c r="I558" s="45" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="559" spans="1:9" customFormat="1" ht="30">
@@ -24785,7 +24786,7 @@
         <v>1062</v>
       </c>
       <c r="C559" s="27" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="D559" s="26"/>
       <c r="E559" s="28" t="s">
@@ -24810,7 +24811,7 @@
         <v>1062</v>
       </c>
       <c r="C560" s="27" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D560" s="26"/>
       <c r="E560" s="28" t="s">
@@ -24835,7 +24836,7 @@
         <v>1062</v>
       </c>
       <c r="C561" s="27" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="D561" s="26"/>
       <c r="E561" s="28" t="s">
@@ -24860,7 +24861,7 @@
         <v>1062</v>
       </c>
       <c r="C562" s="30" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="D562" s="26"/>
       <c r="E562" s="28" t="s">
@@ -25110,7 +25111,7 @@
         <v>1119</v>
       </c>
       <c r="C572" s="30" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="D572" s="26"/>
       <c r="E572" s="28" t="s">
@@ -25135,7 +25136,7 @@
         <v>1062</v>
       </c>
       <c r="C573" s="30" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="D573" s="26"/>
       <c r="E573" s="28" t="s">
@@ -25160,7 +25161,7 @@
         <v>1062</v>
       </c>
       <c r="C574" s="30" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="D574" s="26"/>
       <c r="E574" s="28" t="s">
@@ -25185,7 +25186,7 @@
         <v>1062</v>
       </c>
       <c r="C575" s="30" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="D575" s="26"/>
       <c r="E575" s="28" t="s">
@@ -25210,7 +25211,7 @@
         <v>1062</v>
       </c>
       <c r="C576" s="30" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="D576" s="26"/>
       <c r="E576" s="28" t="s">
@@ -25226,7 +25227,7 @@
         <v>17</v>
       </c>
       <c r="I576" s="45" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="577" spans="1:9" customFormat="1" ht="30">
@@ -25253,7 +25254,7 @@
         <v>17</v>
       </c>
       <c r="I577" s="45" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="578" spans="1:9" customFormat="1" ht="30">
@@ -25314,7 +25315,7 @@
         <v>1062</v>
       </c>
       <c r="C580" s="27" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="D580" s="26"/>
       <c r="E580" s="28" t="s">
@@ -25364,7 +25365,7 @@
         <v>1138</v>
       </c>
       <c r="C582" s="27" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="D582" s="26"/>
       <c r="E582" s="28" t="s">
@@ -25389,7 +25390,7 @@
         <v>1138</v>
       </c>
       <c r="C583" s="30" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D583" s="26"/>
       <c r="E583" s="28" t="s">
@@ -25464,7 +25465,7 @@
         <v>1138</v>
       </c>
       <c r="C586" s="27" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="D586" s="26"/>
       <c r="E586" s="28" t="s">
@@ -25480,7 +25481,7 @@
         <v>17</v>
       </c>
       <c r="I586" s="51" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="587" spans="1:9" customFormat="1" ht="30">
@@ -25491,7 +25492,7 @@
         <v>1138</v>
       </c>
       <c r="C587" s="30" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="D587" s="26"/>
       <c r="E587" s="28" t="s">
@@ -25566,7 +25567,7 @@
         <v>1138</v>
       </c>
       <c r="C590" s="27" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="D590" s="26"/>
       <c r="E590" s="28" t="s">
@@ -25591,7 +25592,7 @@
         <v>1138</v>
       </c>
       <c r="C591" s="27" t="s">
-        <v>1152</v>
+        <v>1588</v>
       </c>
       <c r="D591" s="26"/>
       <c r="E591" s="28" t="s">
@@ -25610,13 +25611,13 @@
     </row>
     <row r="592" spans="1:9" customFormat="1" ht="30">
       <c r="A592" s="25" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B592" s="26" t="s">
         <v>1138</v>
       </c>
       <c r="C592" s="27" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D592" s="26"/>
       <c r="E592" s="28" t="s">
@@ -25635,13 +25636,13 @@
     </row>
     <row r="593" spans="1:9" customFormat="1" ht="30">
       <c r="A593" s="25" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B593" s="26" t="s">
         <v>1138</v>
       </c>
       <c r="C593" s="27" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="D593" s="26"/>
       <c r="E593" s="28" t="s">
@@ -25660,13 +25661,13 @@
     </row>
     <row r="594" spans="1:9" customFormat="1" ht="30">
       <c r="A594" s="25" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B594" s="26" t="s">
         <v>1138</v>
       </c>
       <c r="C594" s="27" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="D594" s="26"/>
       <c r="E594" s="28" t="s">
@@ -25685,13 +25686,13 @@
     </row>
     <row r="595" spans="1:9" customFormat="1" ht="30">
       <c r="A595" s="25" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B595" s="26" t="s">
         <v>1138</v>
       </c>
       <c r="C595" s="27" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D595" s="26"/>
       <c r="E595" s="28" t="s">
@@ -25710,13 +25711,13 @@
     </row>
     <row r="596" spans="1:9" customFormat="1" ht="30">
       <c r="A596" s="25" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B596" s="26" t="s">
         <v>1138</v>
       </c>
       <c r="C596" s="30" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="D596" s="26"/>
       <c r="E596" s="28" t="s">
@@ -25735,13 +25736,13 @@
     </row>
     <row r="597" spans="1:9" customFormat="1" ht="30">
       <c r="A597" s="25" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B597" s="26" t="s">
         <v>1138</v>
       </c>
       <c r="C597" s="27" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D597" s="26"/>
       <c r="E597" s="28" t="s">
@@ -25760,13 +25761,13 @@
     </row>
     <row r="598" spans="1:9" customFormat="1" ht="30">
       <c r="A598" s="25" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B598" s="26" t="s">
         <v>1165</v>
       </c>
-      <c r="B598" s="26" t="s">
+      <c r="C598" s="30" t="s">
         <v>1166</v>
-      </c>
-      <c r="C598" s="30" t="s">
-        <v>1167</v>
       </c>
       <c r="D598" s="26"/>
       <c r="E598" s="28" t="s">
@@ -25785,13 +25786,13 @@
     </row>
     <row r="599" spans="1:9" customFormat="1" ht="105">
       <c r="A599" s="25" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B599" s="26" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C599" s="27" t="s">
         <v>1168</v>
-      </c>
-      <c r="B599" s="26" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C599" s="27" t="s">
-        <v>1169</v>
       </c>
       <c r="D599" s="26"/>
       <c r="E599" s="28" t="s">
@@ -25810,13 +25811,13 @@
     </row>
     <row r="600" spans="1:9" customFormat="1" ht="90">
       <c r="A600" s="25" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B600" s="26" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C600" s="27" t="s">
         <v>1170</v>
-      </c>
-      <c r="B600" s="26" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C600" s="27" t="s">
-        <v>1171</v>
       </c>
       <c r="D600" s="26"/>
       <c r="E600" s="28" t="s">
@@ -25835,13 +25836,13 @@
     </row>
     <row r="601" spans="1:9" customFormat="1" ht="45">
       <c r="A601" s="25" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B601" s="26" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C601" s="27" t="s">
         <v>1172</v>
-      </c>
-      <c r="B601" s="26" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C601" s="27" t="s">
-        <v>1173</v>
       </c>
       <c r="D601" s="26"/>
       <c r="E601" s="28" t="s">
@@ -25860,13 +25861,13 @@
     </row>
     <row r="602" spans="1:9" customFormat="1" ht="45">
       <c r="A602" s="25" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B602" s="26" t="s">
         <v>1174</v>
       </c>
-      <c r="B602" s="26" t="s">
-        <v>1175</v>
-      </c>
       <c r="C602" s="30" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="D602" s="26"/>
       <c r="E602" s="28" t="s">
@@ -25885,13 +25886,13 @@
     </row>
     <row r="603" spans="1:9" customFormat="1" ht="30">
       <c r="A603" s="25" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B603" s="26" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C603" s="30" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="D603" s="26"/>
       <c r="E603" s="28" t="s">
@@ -25910,13 +25911,13 @@
     </row>
     <row r="604" spans="1:9" customFormat="1" ht="30">
       <c r="A604" s="25" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B604" s="26" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C604" s="30" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="D604" s="26"/>
       <c r="E604" s="28" t="s">
@@ -25935,13 +25936,13 @@
     </row>
     <row r="605" spans="1:9" customFormat="1" ht="30">
       <c r="A605" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B605" s="26" t="s">
         <v>1178</v>
       </c>
-      <c r="B605" s="26" t="s">
+      <c r="C605" s="27" t="s">
         <v>1179</v>
-      </c>
-      <c r="C605" s="27" t="s">
-        <v>1180</v>
       </c>
       <c r="D605" s="26"/>
       <c r="E605" s="28" t="s">
@@ -25960,13 +25961,13 @@
     </row>
     <row r="606" spans="1:9" customFormat="1" ht="30">
       <c r="A606" s="25" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B606" s="26" t="s">
         <v>1181</v>
       </c>
-      <c r="B606" s="26" t="s">
+      <c r="C606" s="27" t="s">
         <v>1182</v>
-      </c>
-      <c r="C606" s="27" t="s">
-        <v>1183</v>
       </c>
       <c r="D606" s="26"/>
       <c r="E606" s="28" t="s">
@@ -25985,13 +25986,13 @@
     </row>
     <row r="607" spans="1:9" customFormat="1" ht="30">
       <c r="A607" s="25" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B607" s="26" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C607" s="27" t="s">
         <v>1184</v>
-      </c>
-      <c r="B607" s="26" t="s">
-        <v>1182</v>
-      </c>
-      <c r="C607" s="27" t="s">
-        <v>1185</v>
       </c>
       <c r="D607" s="26"/>
       <c r="E607" s="28" t="s">
@@ -26010,13 +26011,13 @@
     </row>
     <row r="608" spans="1:9" customFormat="1" ht="30">
       <c r="A608" s="25" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B608" s="26" t="s">
         <v>1186</v>
       </c>
-      <c r="B608" s="26" t="s">
+      <c r="C608" s="27" t="s">
         <v>1187</v>
-      </c>
-      <c r="C608" s="27" t="s">
-        <v>1188</v>
       </c>
       <c r="D608" s="26"/>
       <c r="E608" s="28" t="s">
@@ -26035,13 +26036,13 @@
     </row>
     <row r="609" spans="1:9" customFormat="1" ht="30">
       <c r="A609" s="25" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B609" s="26" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C609" s="27" t="s">
         <v>1189</v>
-      </c>
-      <c r="B609" s="26" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C609" s="27" t="s">
-        <v>1190</v>
       </c>
       <c r="D609" s="26"/>
       <c r="E609" s="28" t="s">
@@ -26060,13 +26061,13 @@
     </row>
     <row r="610" spans="1:9" customFormat="1" ht="30">
       <c r="A610" s="25" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B610" s="26" t="s">
         <v>1191</v>
       </c>
-      <c r="B610" s="26" t="s">
+      <c r="C610" s="27" t="s">
         <v>1192</v>
-      </c>
-      <c r="C610" s="27" t="s">
-        <v>1193</v>
       </c>
       <c r="D610" s="26"/>
       <c r="E610" s="28" t="s">
@@ -26085,13 +26086,13 @@
     </row>
     <row r="611" spans="1:9" customFormat="1" ht="45">
       <c r="A611" s="25" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B611" s="26" t="s">
         <v>1194</v>
       </c>
-      <c r="B611" s="26" t="s">
-        <v>1195</v>
-      </c>
       <c r="C611" s="30" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="D611" s="26"/>
       <c r="E611" s="28" t="s">
@@ -26110,13 +26111,13 @@
     </row>
     <row r="612" spans="1:9" customFormat="1" ht="30">
       <c r="A612" s="25" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B612" s="26" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C612" s="30" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="D612" s="26"/>
       <c r="E612" s="28" t="s">
@@ -26135,13 +26136,13 @@
     </row>
     <row r="613" spans="1:9" customFormat="1" ht="30">
       <c r="A613" s="25" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B613" s="26" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C613" s="30" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="D613" s="26"/>
       <c r="E613" s="28" t="s">
@@ -26160,13 +26161,13 @@
     </row>
     <row r="614" spans="1:9" customFormat="1" ht="30">
       <c r="A614" s="25" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B614" s="26" t="s">
         <v>1198</v>
       </c>
-      <c r="B614" s="26" t="s">
+      <c r="C614" s="30" t="s">
         <v>1199</v>
-      </c>
-      <c r="C614" s="30" t="s">
-        <v>1200</v>
       </c>
       <c r="D614" s="26"/>
       <c r="E614" s="28" t="s">
@@ -26185,13 +26186,13 @@
     </row>
     <row r="615" spans="1:9" customFormat="1" ht="120">
       <c r="A615" s="25" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B615" s="26" t="s">
         <v>1201</v>
       </c>
-      <c r="B615" s="26" t="s">
+      <c r="C615" s="30" t="s">
         <v>1202</v>
-      </c>
-      <c r="C615" s="30" t="s">
-        <v>1203</v>
       </c>
       <c r="D615" s="26"/>
       <c r="E615" s="28" t="s">
@@ -26210,13 +26211,13 @@
     </row>
     <row r="616" spans="1:9" customFormat="1" ht="30">
       <c r="A616" s="25" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B616" s="26" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C616" s="27" t="s">
         <v>1204</v>
-      </c>
-      <c r="B616" s="26" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C616" s="27" t="s">
-        <v>1205</v>
       </c>
       <c r="D616" s="26"/>
       <c r="E616" s="28" t="s">
@@ -26235,13 +26236,13 @@
     </row>
     <row r="617" spans="1:9" customFormat="1" ht="30">
       <c r="A617" s="25" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B617" s="26" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C617" s="27" t="s">
         <v>1206</v>
-      </c>
-      <c r="B617" s="26" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C617" s="27" t="s">
-        <v>1207</v>
       </c>
       <c r="D617" s="26"/>
       <c r="E617" s="28" t="s">
@@ -26260,13 +26261,13 @@
     </row>
     <row r="618" spans="1:9" customFormat="1" ht="30">
       <c r="A618" s="25" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B618" s="26" t="s">
         <v>1208</v>
       </c>
-      <c r="B618" s="26" t="s">
+      <c r="C618" s="30" t="s">
         <v>1209</v>
-      </c>
-      <c r="C618" s="30" t="s">
-        <v>1210</v>
       </c>
       <c r="D618" s="26"/>
       <c r="E618" s="28" t="s">
@@ -26285,13 +26286,13 @@
     </row>
     <row r="619" spans="1:9" customFormat="1" ht="150">
       <c r="A619" s="25" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B619" s="26" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C619" s="30" t="s">
         <v>1211</v>
-      </c>
-      <c r="B619" s="26" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C619" s="30" t="s">
-        <v>1212</v>
       </c>
       <c r="D619" s="26"/>
       <c r="E619" s="28" t="s">
@@ -26310,13 +26311,13 @@
     </row>
     <row r="620" spans="1:9" customFormat="1" ht="120">
       <c r="A620" s="25" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B620" s="26" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C620" s="30" t="s">
         <v>1213</v>
-      </c>
-      <c r="B620" s="26" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C620" s="30" t="s">
-        <v>1214</v>
       </c>
       <c r="D620" s="26"/>
       <c r="E620" s="28" t="s">
@@ -26335,13 +26336,13 @@
     </row>
     <row r="621" spans="1:9" customFormat="1" ht="30">
       <c r="A621" s="25" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B621" s="26" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C621" s="30" t="s">
         <v>1215</v>
-      </c>
-      <c r="B621" s="26" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C621" s="30" t="s">
-        <v>1216</v>
       </c>
       <c r="D621" s="26"/>
       <c r="E621" s="28" t="s">
@@ -26360,13 +26361,13 @@
     </row>
     <row r="622" spans="1:9" customFormat="1" ht="30">
       <c r="A622" s="25" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B622" s="26" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C622" s="30" t="s">
         <v>1217</v>
-      </c>
-      <c r="B622" s="26" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C622" s="30" t="s">
-        <v>1218</v>
       </c>
       <c r="D622" s="26"/>
       <c r="E622" s="28" t="s">
@@ -26385,13 +26386,13 @@
     </row>
     <row r="623" spans="1:9" customFormat="1" ht="30">
       <c r="A623" s="25" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B623" s="26" t="s">
         <v>1219</v>
       </c>
-      <c r="B623" s="26" t="s">
+      <c r="C623" s="30" t="s">
         <v>1220</v>
-      </c>
-      <c r="C623" s="30" t="s">
-        <v>1221</v>
       </c>
       <c r="D623" s="26"/>
       <c r="E623" s="28" t="s">
@@ -26410,13 +26411,13 @@
     </row>
     <row r="624" spans="1:9" customFormat="1" ht="90">
       <c r="A624" s="25" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B624" s="26" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C624" s="27" t="s">
         <v>1222</v>
-      </c>
-      <c r="B624" s="26" t="s">
-        <v>1220</v>
-      </c>
-      <c r="C624" s="27" t="s">
-        <v>1223</v>
       </c>
       <c r="D624" s="26"/>
       <c r="E624" s="28" t="s">
@@ -26435,13 +26436,13 @@
     </row>
     <row r="625" spans="1:10" customFormat="1" ht="30">
       <c r="A625" s="25" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B625" s="26" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C625" s="30" t="s">
         <v>1224</v>
-      </c>
-      <c r="B625" s="26" t="s">
-        <v>1220</v>
-      </c>
-      <c r="C625" s="30" t="s">
-        <v>1225</v>
       </c>
       <c r="D625" s="26"/>
       <c r="E625" s="28" t="s">
@@ -26460,13 +26461,13 @@
     </row>
     <row r="626" spans="1:10" customFormat="1" ht="30">
       <c r="A626" s="25" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B626" s="26" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C626" s="27" t="s">
         <v>1226</v>
-      </c>
-      <c r="B626" s="26" t="s">
-        <v>1220</v>
-      </c>
-      <c r="C626" s="27" t="s">
-        <v>1227</v>
       </c>
       <c r="D626" s="26"/>
       <c r="E626" s="28" t="s">
@@ -26485,13 +26486,13 @@
     </row>
     <row r="627" spans="1:10" customFormat="1" ht="30">
       <c r="A627" s="25" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B627" s="26" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C627" s="27" t="s">
         <v>1228</v>
-      </c>
-      <c r="B627" s="26" t="s">
-        <v>1220</v>
-      </c>
-      <c r="C627" s="27" t="s">
-        <v>1229</v>
       </c>
       <c r="D627" s="26"/>
       <c r="E627" s="28" t="s">
@@ -26510,13 +26511,13 @@
     </row>
     <row r="628" spans="1:10" customFormat="1" ht="30">
       <c r="A628" s="25" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B628" s="26" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C628" s="27" t="s">
         <v>1230</v>
-      </c>
-      <c r="B628" s="26" t="s">
-        <v>1220</v>
-      </c>
-      <c r="C628" s="27" t="s">
-        <v>1231</v>
       </c>
       <c r="D628" s="26"/>
       <c r="E628" s="28" t="s">
@@ -26536,13 +26537,13 @@
     </row>
     <row r="629" spans="1:10" customFormat="1" ht="30">
       <c r="A629" s="25" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B629" s="26" t="s">
         <v>1232</v>
       </c>
-      <c r="B629" s="26" t="s">
+      <c r="C629" s="27" t="s">
         <v>1233</v>
-      </c>
-      <c r="C629" s="27" t="s">
-        <v>1234</v>
       </c>
       <c r="D629" s="26"/>
       <c r="E629" s="28" t="s">
@@ -26561,13 +26562,13 @@
     </row>
     <row r="630" spans="1:10" customFormat="1" ht="45">
       <c r="A630" s="25" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B630" s="26" t="s">
         <v>1235</v>
       </c>
-      <c r="B630" s="26" t="s">
-        <v>1236</v>
-      </c>
       <c r="C630" s="30" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="D630" s="26"/>
       <c r="E630" s="28" t="s">
@@ -26586,13 +26587,13 @@
     </row>
     <row r="631" spans="1:10" customFormat="1" ht="30">
       <c r="A631" s="25" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B631" s="26" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C631" s="30" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="D631" s="26"/>
       <c r="E631" s="28" t="s">
@@ -26611,13 +26612,13 @@
     </row>
     <row r="632" spans="1:10" customFormat="1" ht="30">
       <c r="A632" s="25" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B632" s="26" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C632" s="30" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="D632" s="26"/>
       <c r="E632" s="28" t="s">
@@ -26636,13 +26637,13 @@
     </row>
     <row r="633" spans="1:10" customFormat="1" ht="45">
       <c r="A633" s="25" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B633" s="26" t="s">
         <v>1239</v>
       </c>
-      <c r="B633" s="26" t="s">
+      <c r="C633" s="27" t="s">
         <v>1240</v>
-      </c>
-      <c r="C633" s="27" t="s">
-        <v>1241</v>
       </c>
       <c r="D633" s="26"/>
       <c r="E633" s="28" t="s">
@@ -26661,13 +26662,13 @@
     </row>
     <row r="634" spans="1:10" customFormat="1" ht="45">
       <c r="A634" s="25" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B634" s="26" t="s">
         <v>1242</v>
       </c>
-      <c r="B634" s="26" t="s">
+      <c r="C634" s="27" t="s">
         <v>1243</v>
-      </c>
-      <c r="C634" s="27" t="s">
-        <v>1244</v>
       </c>
       <c r="D634" s="26"/>
       <c r="E634" s="28" t="s">
@@ -26686,13 +26687,13 @@
     </row>
     <row r="635" spans="1:10" customFormat="1" ht="45">
       <c r="A635" s="25" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B635" s="26" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C635" s="27" t="s">
         <v>1245</v>
-      </c>
-      <c r="B635" s="26" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C635" s="27" t="s">
-        <v>1246</v>
       </c>
       <c r="D635" s="26"/>
       <c r="E635" s="28" t="s">
@@ -26711,13 +26712,13 @@
     </row>
     <row r="636" spans="1:10" customFormat="1" ht="45">
       <c r="A636" s="25" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B636" s="26" t="s">
         <v>1247</v>
       </c>
-      <c r="B636" s="26" t="s">
+      <c r="C636" s="27" t="s">
         <v>1248</v>
-      </c>
-      <c r="C636" s="27" t="s">
-        <v>1249</v>
       </c>
       <c r="D636" s="26"/>
       <c r="E636" s="28" t="s">
@@ -26736,13 +26737,13 @@
     </row>
     <row r="637" spans="1:10" customFormat="1" ht="45">
       <c r="A637" s="25" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B637" s="26" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C637" s="27" t="s">
         <v>1250</v>
-      </c>
-      <c r="B637" s="26" t="s">
-        <v>1248</v>
-      </c>
-      <c r="C637" s="27" t="s">
-        <v>1251</v>
       </c>
       <c r="D637" s="26"/>
       <c r="E637" s="28" t="s">
@@ -26761,13 +26762,13 @@
     </row>
     <row r="638" spans="1:10" customFormat="1" ht="45">
       <c r="A638" s="25" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B638" s="26" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C638" s="27" t="s">
         <v>1252</v>
-      </c>
-      <c r="B638" s="26" t="s">
-        <v>1248</v>
-      </c>
-      <c r="C638" s="27" t="s">
-        <v>1253</v>
       </c>
       <c r="D638" s="26"/>
       <c r="E638" s="28" t="s">
@@ -26786,13 +26787,13 @@
     </row>
     <row r="639" spans="1:10" customFormat="1" ht="45">
       <c r="A639" s="25" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B639" s="26" t="s">
         <v>1254</v>
       </c>
-      <c r="B639" s="26" t="s">
-        <v>1255</v>
-      </c>
       <c r="C639" s="30" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="D639" s="26"/>
       <c r="E639" s="28" t="s">
@@ -26811,13 +26812,13 @@
     </row>
     <row r="640" spans="1:10" customFormat="1" ht="30">
       <c r="A640" s="25" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B640" s="26" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="C640" s="30" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="D640" s="26"/>
       <c r="E640" s="28" t="s">
@@ -26836,13 +26837,13 @@
     </row>
     <row r="641" spans="1:9" customFormat="1" ht="30">
       <c r="A641" s="25" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B641" s="26" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="C641" s="30" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="D641" s="26"/>
       <c r="E641" s="28" t="s">
@@ -26861,13 +26862,13 @@
     </row>
     <row r="642" spans="1:9" customFormat="1" ht="45">
       <c r="A642" s="25" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B642" s="26" t="s">
         <v>1258</v>
       </c>
-      <c r="B642" s="26" t="s">
+      <c r="C642" s="30" t="s">
         <v>1259</v>
-      </c>
-      <c r="C642" s="30" t="s">
-        <v>1260</v>
       </c>
       <c r="D642" s="26"/>
       <c r="E642" s="28" t="s">
@@ -26886,13 +26887,13 @@
     </row>
     <row r="643" spans="1:9" customFormat="1" ht="120">
       <c r="A643" s="25" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B643" s="26" t="s">
         <v>1261</v>
       </c>
-      <c r="B643" s="26" t="s">
+      <c r="C643" s="30" t="s">
         <v>1262</v>
-      </c>
-      <c r="C643" s="30" t="s">
-        <v>1263</v>
       </c>
       <c r="D643" s="26"/>
       <c r="E643" s="28" t="s">
@@ -26911,13 +26912,13 @@
     </row>
     <row r="644" spans="1:9" customFormat="1" ht="45">
       <c r="A644" s="25" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B644" s="26" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C644" s="27" t="s">
         <v>1264</v>
-      </c>
-      <c r="B644" s="26" t="s">
-        <v>1262</v>
-      </c>
-      <c r="C644" s="27" t="s">
-        <v>1265</v>
       </c>
       <c r="D644" s="26"/>
       <c r="E644" s="28" t="s">
@@ -26936,13 +26937,13 @@
     </row>
     <row r="645" spans="1:9" customFormat="1" ht="45">
       <c r="A645" s="25" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B645" s="26" t="s">
         <v>1266</v>
       </c>
-      <c r="B645" s="26" t="s">
+      <c r="C645" s="30" t="s">
         <v>1267</v>
-      </c>
-      <c r="C645" s="30" t="s">
-        <v>1268</v>
       </c>
       <c r="D645" s="26"/>
       <c r="E645" s="28" t="s">
@@ -26961,13 +26962,13 @@
     </row>
     <row r="646" spans="1:9" customFormat="1" ht="120">
       <c r="A646" s="25" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B646" s="26" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C646" s="30" t="s">
         <v>1269</v>
-      </c>
-      <c r="B646" s="26" t="s">
-        <v>1267</v>
-      </c>
-      <c r="C646" s="30" t="s">
-        <v>1270</v>
       </c>
       <c r="D646" s="26"/>
       <c r="E646" s="28" t="s">
@@ -26986,13 +26987,13 @@
     </row>
     <row r="647" spans="1:9" customFormat="1" ht="120">
       <c r="A647" s="25" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B647" s="26" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C647" s="30" t="s">
         <v>1271</v>
-      </c>
-      <c r="B647" s="26" t="s">
-        <v>1267</v>
-      </c>
-      <c r="C647" s="30" t="s">
-        <v>1272</v>
       </c>
       <c r="D647" s="26"/>
       <c r="E647" s="28" t="s">
@@ -27011,13 +27012,13 @@
     </row>
     <row r="648" spans="1:9" customFormat="1" ht="45">
       <c r="A648" s="25" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B648" s="26" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C648" s="27" t="s">
         <v>1273</v>
-      </c>
-      <c r="B648" s="26" t="s">
-        <v>1267</v>
-      </c>
-      <c r="C648" s="27" t="s">
-        <v>1274</v>
       </c>
       <c r="D648" s="26"/>
       <c r="E648" s="28" t="s">
@@ -27036,13 +27037,13 @@
     </row>
     <row r="649" spans="1:9" customFormat="1" ht="45">
       <c r="A649" s="25" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B649" s="26" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C649" s="27" t="s">
         <v>1275</v>
-      </c>
-      <c r="B649" s="26" t="s">
-        <v>1267</v>
-      </c>
-      <c r="C649" s="27" t="s">
-        <v>1276</v>
       </c>
       <c r="D649" s="26"/>
       <c r="E649" s="28" t="s">
@@ -27061,13 +27062,13 @@
     </row>
     <row r="650" spans="1:9" customFormat="1" ht="30">
       <c r="A650" s="25" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B650" s="26" t="s">
         <v>1277</v>
       </c>
-      <c r="B650" s="26" t="s">
+      <c r="C650" s="30" t="s">
         <v>1278</v>
-      </c>
-      <c r="C650" s="30" t="s">
-        <v>1279</v>
       </c>
       <c r="D650" s="26"/>
       <c r="E650" s="28" t="s">
@@ -27086,13 +27087,13 @@
     </row>
     <row r="651" spans="1:9" customFormat="1" ht="30">
       <c r="A651" s="25" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B651" s="26" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="C651" s="30" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="D651" s="26"/>
       <c r="E651" s="28" t="s">
@@ -27111,13 +27112,13 @@
     </row>
     <row r="652" spans="1:9" customFormat="1" ht="105">
       <c r="A652" s="25" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B652" s="26" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C652" s="30" t="s">
         <v>1281</v>
-      </c>
-      <c r="B652" s="26" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C652" s="30" t="s">
-        <v>1282</v>
       </c>
       <c r="D652" s="26"/>
       <c r="E652" s="28" t="s">
@@ -27136,13 +27137,13 @@
     </row>
     <row r="653" spans="1:9" customFormat="1" ht="30">
       <c r="A653" s="25" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B653" s="26" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C653" s="27" t="s">
         <v>1283</v>
-      </c>
-      <c r="B653" s="26" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C653" s="27" t="s">
-        <v>1284</v>
       </c>
       <c r="D653" s="26"/>
       <c r="E653" s="28" t="s">
@@ -27161,13 +27162,13 @@
     </row>
     <row r="654" spans="1:9" customFormat="1" ht="30">
       <c r="A654" s="25" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B654" s="26" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C654" s="30" t="s">
         <v>1285</v>
-      </c>
-      <c r="B654" s="26" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C654" s="30" t="s">
-        <v>1286</v>
       </c>
       <c r="D654" s="26"/>
       <c r="E654" s="28" t="s">
@@ -27186,13 +27187,13 @@
     </row>
     <row r="655" spans="1:9" customFormat="1" ht="45">
       <c r="A655" s="25" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B655" s="26" t="s">
         <v>1287</v>
       </c>
-      <c r="B655" s="26" t="s">
-        <v>1288</v>
-      </c>
       <c r="C655" s="30" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D655" s="26"/>
       <c r="E655" s="28" t="s">
@@ -27211,13 +27212,13 @@
     </row>
     <row r="656" spans="1:9" customFormat="1" ht="30">
       <c r="A656" s="25" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B656" s="26" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="C656" s="30" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="D656" s="26"/>
       <c r="E656" s="28" t="s">
@@ -27236,13 +27237,13 @@
     </row>
     <row r="657" spans="1:9" customFormat="1" ht="30">
       <c r="A657" s="25" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B657" s="26" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="C657" s="30" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="D657" s="26"/>
       <c r="E657" s="28" t="s">
@@ -27261,13 +27262,13 @@
     </row>
     <row r="658" spans="1:9" customFormat="1" ht="45">
       <c r="A658" s="25" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B658" s="26" t="s">
         <v>1291</v>
       </c>
-      <c r="B658" s="26" t="s">
+      <c r="C658" s="27" t="s">
         <v>1292</v>
-      </c>
-      <c r="C658" s="27" t="s">
-        <v>1293</v>
       </c>
       <c r="D658" s="26"/>
       <c r="E658" s="28" t="s">
@@ -27286,13 +27287,13 @@
     </row>
     <row r="659" spans="1:9" customFormat="1" ht="45">
       <c r="A659" s="25" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B659" s="26" t="s">
         <v>1294</v>
       </c>
-      <c r="B659" s="26" t="s">
+      <c r="C659" s="27" t="s">
         <v>1295</v>
-      </c>
-      <c r="C659" s="27" t="s">
-        <v>1296</v>
       </c>
       <c r="D659" s="26"/>
       <c r="E659" s="28" t="s">
@@ -27311,13 +27312,13 @@
     </row>
     <row r="660" spans="1:9" customFormat="1" ht="45">
       <c r="A660" s="25" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B660" s="26" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C660" s="27" t="s">
         <v>1297</v>
-      </c>
-      <c r="B660" s="26" t="s">
-        <v>1295</v>
-      </c>
-      <c r="C660" s="27" t="s">
-        <v>1298</v>
       </c>
       <c r="D660" s="26"/>
       <c r="E660" s="28" t="s">
@@ -27336,13 +27337,13 @@
     </row>
     <row r="661" spans="1:9" customFormat="1" ht="45">
       <c r="A661" s="25" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B661" s="26" t="s">
         <v>1299</v>
       </c>
-      <c r="B661" s="26" t="s">
+      <c r="C661" s="27" t="s">
         <v>1300</v>
-      </c>
-      <c r="C661" s="27" t="s">
-        <v>1301</v>
       </c>
       <c r="D661" s="26"/>
       <c r="E661" s="28" t="s">
@@ -27361,13 +27362,13 @@
     </row>
     <row r="662" spans="1:9" customFormat="1" ht="45">
       <c r="A662" s="25" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B662" s="26" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C662" s="27" t="s">
         <v>1302</v>
-      </c>
-      <c r="B662" s="26" t="s">
-        <v>1300</v>
-      </c>
-      <c r="C662" s="27" t="s">
-        <v>1303</v>
       </c>
       <c r="D662" s="26"/>
       <c r="E662" s="28" t="s">
@@ -27386,13 +27387,13 @@
     </row>
     <row r="663" spans="1:9" customFormat="1" ht="45">
       <c r="A663" s="25" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B663" s="26" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C663" s="27" t="s">
         <v>1304</v>
-      </c>
-      <c r="B663" s="26" t="s">
-        <v>1300</v>
-      </c>
-      <c r="C663" s="27" t="s">
-        <v>1305</v>
       </c>
       <c r="D663" s="26"/>
       <c r="E663" s="28" t="s">
@@ -27411,13 +27412,13 @@
     </row>
     <row r="664" spans="1:9" customFormat="1" ht="45">
       <c r="A664" s="25" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B664" s="26" t="s">
         <v>1306</v>
       </c>
-      <c r="B664" s="26" t="s">
-        <v>1307</v>
-      </c>
       <c r="C664" s="30" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="D664" s="26"/>
       <c r="E664" s="28" t="s">
@@ -27436,13 +27437,13 @@
     </row>
     <row r="665" spans="1:9" customFormat="1" ht="30">
       <c r="A665" s="25" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B665" s="26" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C665" s="30" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D665" s="26"/>
       <c r="E665" s="28" t="s">
@@ -27461,13 +27462,13 @@
     </row>
     <row r="666" spans="1:9" customFormat="1" ht="30">
       <c r="A666" s="25" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B666" s="26" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C666" s="30" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="D666" s="26"/>
       <c r="E666" s="28" t="s">
@@ -27486,13 +27487,13 @@
     </row>
     <row r="667" spans="1:9" customFormat="1" ht="45">
       <c r="A667" s="25" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B667" s="26" t="s">
         <v>1310</v>
       </c>
-      <c r="B667" s="26" t="s">
+      <c r="C667" s="30" t="s">
         <v>1311</v>
-      </c>
-      <c r="C667" s="30" t="s">
-        <v>1312</v>
       </c>
       <c r="D667" s="26"/>
       <c r="E667" s="28" t="s">
@@ -27511,13 +27512,13 @@
     </row>
     <row r="668" spans="1:9" customFormat="1" ht="135">
       <c r="A668" s="25" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B668" s="26" t="s">
         <v>1313</v>
       </c>
-      <c r="B668" s="26" t="s">
+      <c r="C668" s="30" t="s">
         <v>1314</v>
-      </c>
-      <c r="C668" s="30" t="s">
-        <v>1315</v>
       </c>
       <c r="D668" s="26"/>
       <c r="E668" s="28" t="s">
@@ -27536,13 +27537,13 @@
     </row>
     <row r="669" spans="1:9" customFormat="1" ht="75">
       <c r="A669" s="25" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="B669" s="26" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C669" s="30" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="D669" s="26"/>
       <c r="E669" s="28" t="s">
@@ -27561,13 +27562,13 @@
     </row>
     <row r="670" spans="1:9" customFormat="1" ht="45">
       <c r="A670" s="25" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B670" s="26" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C670" s="30" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="D670" s="26"/>
       <c r="E670" s="28" t="s">
@@ -27586,13 +27587,13 @@
     </row>
     <row r="671" spans="1:9" customFormat="1" ht="45">
       <c r="A671" s="25" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B671" s="26" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C671" s="30" t="s">
         <v>1318</v>
-      </c>
-      <c r="B671" s="26" t="s">
-        <v>1314</v>
-      </c>
-      <c r="C671" s="30" t="s">
-        <v>1319</v>
       </c>
       <c r="D671" s="26"/>
       <c r="E671" s="28" t="s">
@@ -27611,13 +27612,13 @@
     </row>
     <row r="672" spans="1:9" customFormat="1" ht="45">
       <c r="A672" s="25" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B672" s="26" t="s">
         <v>1320</v>
       </c>
-      <c r="B672" s="26" t="s">
+      <c r="C672" s="30" t="s">
         <v>1321</v>
-      </c>
-      <c r="C672" s="30" t="s">
-        <v>1322</v>
       </c>
       <c r="D672" s="26"/>
       <c r="E672" s="28" t="s">
@@ -27636,13 +27637,13 @@
     </row>
     <row r="673" spans="1:9" customFormat="1" ht="120">
       <c r="A673" s="25" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B673" s="26" t="s">
         <v>1323</v>
       </c>
-      <c r="B673" s="26" t="s">
-        <v>1324</v>
-      </c>
       <c r="C673" s="30" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="D673" s="26"/>
       <c r="E673" s="28" t="s">
@@ -27661,13 +27662,13 @@
     </row>
     <row r="674" spans="1:9" customFormat="1" ht="45">
       <c r="A674" s="25" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B674" s="26" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C674" s="27" t="s">
         <v>1325</v>
-      </c>
-      <c r="B674" s="26" t="s">
-        <v>1321</v>
-      </c>
-      <c r="C674" s="27" t="s">
-        <v>1326</v>
       </c>
       <c r="D674" s="26"/>
       <c r="E674" s="28" t="s">
@@ -27686,13 +27687,13 @@
     </row>
     <row r="675" spans="1:9" customFormat="1" ht="45">
       <c r="A675" s="25" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B675" s="26" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C675" s="27" t="s">
         <v>1327</v>
-      </c>
-      <c r="B675" s="26" t="s">
-        <v>1321</v>
-      </c>
-      <c r="C675" s="27" t="s">
-        <v>1328</v>
       </c>
       <c r="D675" s="26"/>
       <c r="E675" s="28" t="s">
@@ -27711,13 +27712,13 @@
     </row>
     <row r="676" spans="1:9" customFormat="1" ht="45">
       <c r="A676" s="25" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B676" s="26" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C676" s="30" t="s">
         <v>1329</v>
-      </c>
-      <c r="B676" s="26" t="s">
-        <v>1324</v>
-      </c>
-      <c r="C676" s="30" t="s">
-        <v>1330</v>
       </c>
       <c r="D676" s="26"/>
       <c r="E676" s="28" t="s">
@@ -27736,13 +27737,13 @@
     </row>
     <row r="677" spans="1:9" customFormat="1" ht="60">
       <c r="A677" s="25" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B677" s="26" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C677" s="30" t="s">
         <v>1331</v>
-      </c>
-      <c r="B677" s="26" t="s">
-        <v>1324</v>
-      </c>
-      <c r="C677" s="30" t="s">
-        <v>1332</v>
       </c>
       <c r="D677" s="26"/>
       <c r="E677" s="28" t="s">
@@ -27761,10 +27762,10 @@
     </row>
     <row r="678" spans="1:9" customFormat="1" ht="45">
       <c r="A678" s="25" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B678" s="26" t="s">
         <v>1333</v>
-      </c>
-      <c r="B678" s="26" t="s">
-        <v>1334</v>
       </c>
       <c r="C678" s="30" t="s">
         <v>1587</v>
@@ -27786,13 +27787,13 @@
     </row>
     <row r="679" spans="1:9" customFormat="1" ht="30">
       <c r="A679" s="25" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B679" s="26" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C679" s="30" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="D679" s="26"/>
       <c r="E679" s="28" t="s">
@@ -27814,10 +27815,10 @@
         <v>60</v>
       </c>
       <c r="B680" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C680" s="47" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D680" s="41" t="s">
         <v>61</v>
@@ -27835,7 +27836,7 @@
         <v>21</v>
       </c>
       <c r="I680" s="50" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="681" spans="1:9" s="39" customFormat="1" ht="60">
@@ -27843,13 +27844,13 @@
         <v>480</v>
       </c>
       <c r="B681" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C681" s="47" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="D681" s="41" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="E681" s="42" t="s">
         <v>22</v>
@@ -27864,7 +27865,7 @@
         <v>20</v>
       </c>
       <c r="I681" s="45" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="682" spans="1:9" s="39" customFormat="1" ht="60">
@@ -27872,10 +27873,10 @@
         <v>809</v>
       </c>
       <c r="B682" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C682" s="47" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="D682" s="41" t="s">
         <v>810</v>
@@ -27893,7 +27894,7 @@
         <v>20</v>
       </c>
       <c r="I682" s="45" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="683" spans="1:9" s="39" customFormat="1" ht="60">
@@ -27901,10 +27902,10 @@
         <v>858</v>
       </c>
       <c r="B683" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C683" s="47" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="D683" s="41" t="s">
         <v>859</v>
@@ -27922,7 +27923,7 @@
         <v>20</v>
       </c>
       <c r="I683" s="45" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="684" spans="1:9" s="39" customFormat="1" ht="60">
@@ -27930,10 +27931,10 @@
         <v>1080</v>
       </c>
       <c r="B684" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C684" s="47" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="D684" s="41" t="s">
         <v>1081</v>
@@ -27951,7 +27952,7 @@
         <v>20</v>
       </c>
       <c r="I684" s="45" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="685" spans="1:9" s="39" customFormat="1" ht="60">
@@ -27959,13 +27960,13 @@
         <v>1128</v>
       </c>
       <c r="B685" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C685" s="47" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="D685" s="41" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="E685" s="42" t="s">
         <v>22</v>
@@ -27980,7 +27981,7 @@
         <v>20</v>
       </c>
       <c r="I685" s="45" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="686" spans="1:9" s="39" customFormat="1" ht="60">
@@ -27988,13 +27989,13 @@
         <v>1129</v>
       </c>
       <c r="B686" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C686" s="47" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="D686" s="41" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="E686" s="42" t="s">
         <v>22</v>
@@ -28009,21 +28010,21 @@
         <v>20</v>
       </c>
       <c r="I686" s="45" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="687" spans="1:9" customFormat="1" ht="45">
       <c r="A687" s="25" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B687" s="26" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C687" s="45" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D687" s="41" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E687" s="28" t="s">
         <v>22</v>
@@ -28041,16 +28042,16 @@
     </row>
     <row r="688" spans="1:9" customFormat="1" ht="45">
       <c r="A688" s="25" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B688" s="26" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C688" s="33" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="D688" s="41" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="E688" s="28" t="s">
         <v>22</v>
@@ -28068,16 +28069,16 @@
     </row>
     <row r="689" spans="1:9" customFormat="1" ht="60">
       <c r="A689" s="25" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B689" s="26" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C689" s="49" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="D689" s="41" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="E689" s="28" t="s">
         <v>22</v>
@@ -28095,16 +28096,16 @@
     </row>
     <row r="690" spans="1:9" s="38" customFormat="1" ht="75">
       <c r="A690" s="40" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B690" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C690" s="45" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="D690" s="41" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="E690" s="42" t="s">
         <v>22</v>
@@ -28119,18 +28120,18 @@
         <v>20</v>
       </c>
       <c r="I690" s="35" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="691" spans="1:9" customFormat="1" ht="60">
       <c r="A691" s="25" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B691" s="26" t="s">
         <v>1339</v>
       </c>
-      <c r="B691" s="26" t="s">
-        <v>1340</v>
-      </c>
       <c r="C691" s="45" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="D691" s="41"/>
       <c r="E691" s="28" t="s">
@@ -28152,13 +28153,13 @@
         <v>690</v>
       </c>
       <c r="B692" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C692" s="47" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="D692" s="36" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="E692" s="55" t="s">
         <v>22</v>
@@ -28173,21 +28174,21 @@
         <v>20</v>
       </c>
       <c r="I692" s="35" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="693" spans="1:9" s="39" customFormat="1" ht="60">
       <c r="A693" s="40" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B693" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C693" s="48" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="D693" s="36" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="E693" s="55" t="s">
         <v>22</v>
@@ -28202,21 +28203,21 @@
         <v>20</v>
       </c>
       <c r="I693" s="35" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="694" spans="1:9" s="39" customFormat="1" ht="60">
       <c r="A694" s="40" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B694" s="41" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C694" s="48" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="D694" s="36" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="E694" s="55" t="s">
         <v>22</v>
@@ -28231,21 +28232,21 @@
         <v>20</v>
       </c>
       <c r="I694" s="35" t="s">
-        <v>1349</v>
-      </c>
-    </row>
-    <row r="695" spans="1:9" customFormat="1" ht="105">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="695" spans="1:9" customFormat="1" ht="90">
       <c r="A695" s="25" t="s">
         <v>1585</v>
       </c>
       <c r="B695" s="26" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="C695" s="45" t="s">
-        <v>1588</v>
+        <v>1582</v>
       </c>
       <c r="D695" s="36" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="E695" s="28" t="s">
         <v>22</v>
@@ -28260,21 +28261,21 @@
         <v>20</v>
       </c>
       <c r="I695" s="54" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="696" spans="1:9" s="39" customFormat="1" ht="45">
       <c r="A696" s="59" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="B696" s="36" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C696" s="45" t="s">
         <v>1586</v>
       </c>
       <c r="D696" s="36" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="E696" s="42" t="s">
         <v>22</v>
@@ -28292,16 +28293,16 @@
     </row>
     <row r="697" spans="1:9" s="39" customFormat="1" ht="90">
       <c r="A697" s="60" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B697" s="53" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C697" s="45" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="D697" s="36" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="E697" s="42" t="s">
         <v>22</v>
@@ -28316,21 +28317,21 @@
         <v>20</v>
       </c>
       <c r="I697" s="35" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="698" spans="1:9" s="39" customFormat="1" ht="45">
       <c r="A698" s="61" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B698" s="36" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C698" s="54" t="s">
         <v>1547</v>
       </c>
-      <c r="B698" s="36" t="s">
-        <v>1334</v>
-      </c>
-      <c r="C698" s="54" t="s">
+      <c r="D698" s="36" t="s">
         <v>1548</v>
-      </c>
-      <c r="D698" s="36" t="s">
-        <v>1549</v>
       </c>
       <c r="E698" s="42" t="s">
         <v>22</v>
@@ -28348,16 +28349,16 @@
     </row>
     <row r="699" spans="1:9" s="39" customFormat="1" ht="45">
       <c r="A699" s="61" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="B699" s="36" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C699" s="54" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D699" s="36" t="s">
         <v>1563</v>
-      </c>
-      <c r="D699" s="36" t="s">
-        <v>1564</v>
       </c>
       <c r="E699" s="42" t="s">
         <v>22</v>
@@ -28372,21 +28373,21 @@
         <v>21</v>
       </c>
       <c r="I699" s="57" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="700" spans="1:9" s="39" customFormat="1" ht="45">
       <c r="A700" s="61" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B700" s="36" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C700" s="54" t="s">
         <v>1566</v>
       </c>
-      <c r="B700" s="36" t="s">
-        <v>1334</v>
-      </c>
-      <c r="C700" s="54" t="s">
-        <v>1567</v>
-      </c>
       <c r="D700" s="36" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="E700" s="42" t="s">
         <v>22</v>
@@ -28401,18 +28402,18 @@
         <v>21</v>
       </c>
       <c r="I700" s="57" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="701" spans="1:9" customFormat="1" ht="30">
       <c r="A701" s="25" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B701" s="26" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C701" s="45" t="s">
         <v>1558</v>
-      </c>
-      <c r="B701" s="26" t="s">
-        <v>1340</v>
-      </c>
-      <c r="C701" s="45" t="s">
-        <v>1559</v>
       </c>
       <c r="D701" s="26"/>
       <c r="E701" s="28" t="s">
@@ -28435,6 +28436,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -28442,11 +28448,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A577:B577 I619:I622 I678:I679 A293:B293 A513:C513 A116:C128 A131:C141 A516:C521 D524 A115:G115 A227:D227 A689:B690 I199 A687:C688 A691:C691 A239:C292 I41:I63 A309:I341 B168:D169 I168:I169 D294:H294 D116:H141 D576:D577 D523:E523 A143:I149 A343:I352 A151:I154 A150:H150 A156:I157 A155:H155 A159:I161 A158:H158 A228:H238 A525:D525 A528:D528 A142:H142 A342:H342 E655:I662 E654:H654 E664:I672 E663:H663 E674:I675 E673:H673 E676:H679 D516:H522 A514:D515 A195:H195 A353:H353 D239:I293 A20:H114 A163:I163 A162:H162 E623:I653 A295:I307 A308:H308 A354:I460 A578:D679 A701:D701 A170:I193 A692:D694 A684:D684 A681:I683 A680:H680 B164:I164 E165:H169 A197:H226 A463:I486 I496:I514 A487:D512 E487:H514 I538:I544 A531:D575 E525:H622 A695:C700 E684:H701 I546:I561">
@@ -30940,12 +30941,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30998,15 +30996,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -31027,15 +31034,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update md and RS file for MS-DWSS
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-DWSS/MS-DWSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-DWSS/MS-DWSS_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FF6C67-E60E-4A6A-A32A-9902BDAE08CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB798A74-CFD5-4AFA-8A13-B2EAD3E8D8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21105" windowHeight="12480" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -6403,6 +6403,21 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6426,21 +6441,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10877,7 +10877,7 @@
   <dimension ref="A1:L702"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B5" sqref="B5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -10927,132 +10927,132 @@
         <v>1455</v>
       </c>
       <c r="F3" s="13">
-        <v>44397</v>
+        <v>44516</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -11065,12 +11065,12 @@
       <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -11083,12 +11083,12 @@
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -11101,12 +11101,12 @@
       <c r="C14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -11119,60 +11119,60 @@
       <c r="C15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="81" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="73" t="s">
         <v>1454</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -28436,11 +28436,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -28448,6 +28443,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A577:B577 I619:I622 I678:I679 A293:B293 A513:C513 A116:C128 A131:C141 A516:C521 D524 A115:G115 A227:D227 A689:B690 I199 A687:C688 A691:C691 A239:C292 I41:I63 A309:I341 B168:D169 I168:I169 D294:H294 D116:H141 D576:D577 D523:E523 A143:I149 A343:I352 A151:I154 A150:H150 A156:I157 A155:H155 A159:I161 A158:H158 A228:H238 A525:D525 A528:D528 A142:H142 A342:H342 E655:I662 E654:H654 E664:I672 E663:H663 E674:I675 E673:H673 E676:H679 D516:H522 A514:D515 A195:H195 A353:H353 D239:I293 A20:H114 A163:I163 A162:H162 E623:I653 A295:I307 A308:H308 A354:I460 A578:D679 A701:D701 A170:I193 A692:D694 A684:D684 A681:I683 A680:H680 B164:I164 E165:H169 A197:H226 A463:I486 I496:I514 A487:D512 E487:H514 I538:I544 A531:D575 E525:H622 A695:C700 E684:H701 I546:I561">
@@ -30947,6 +30947,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -30995,15 +31004,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -31019,6 +31019,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31031,12 +31039,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-DWSS updated RS and xml files.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-DWSS/MS-DWSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-DWSS/MS-DWSS_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1815E3B6-5C76-4EBD-8774-3F66B3AB32CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853C66CB-2CBA-4609-92C1-76DC647CF789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-1272" windowWidth="23256" windowHeight="12456" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5983,10 +5983,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] Implementation does return HTTP status code 401 with response body which contains text "401 Unauthorized" instead of the "NoAccess" error if the authenticated user is not permitted to access this information. (Windows SharePoint Services 3.0, SharePoint Foundation 2010, SharePoint Foundation 2013, and SharePoint Server 2016 will never return the "NoAccess" error code; instead, these product versions will return HTTP status code 401 with a response body containing the text "401 Unauthorized".)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MS-DWSS_R4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6020,6 +6016,9 @@
   </si>
   <si>
     <t>15.4</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does return HTTP status code 401 with response body which contains text "401 Unauthorized" instead of the "NoAccess" error if the authenticated user is not permitted to access this information. (Windows SharePoint Services 3.0, SharePoint Foundation 2010, SharePoint Foundation 2013, SharePoint Server 2016 and SharePoint Server 2019 will never return the "NoAccess" error code; instead, these product versions will return HTTP status code 401 with a response body containing the text "401 Unauthorized".)</t>
   </si>
 </sst>
 </file>
@@ -6384,21 +6383,6 @@
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6422,6 +6406,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10857,8 +10856,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J703"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:I7"/>
+    <sheetView tabSelected="1" topLeftCell="A693" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C696" sqref="C696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -10901,7 +10900,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>1455</v>
@@ -10912,127 +10911,127 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
@@ -11045,12 +11044,12 @@
       <c r="C12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -11063,12 +11062,12 @@
       <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10">
@@ -11081,12 +11080,12 @@
       <c r="C14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10">
@@ -11099,60 +11098,60 @@
       <c r="C15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="81" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="53" t="s">
         <v>1454</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="28.8">
@@ -11438,7 +11437,7 @@
     </row>
     <row r="30" spans="1:10" customFormat="1" ht="28.8">
       <c r="A30" s="22" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B30" s="23" t="s">
         <v>56</v>
@@ -11463,7 +11462,7 @@
     </row>
     <row r="31" spans="1:10" customFormat="1" ht="43.2">
       <c r="A31" s="22" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="B31" s="23" t="s">
         <v>56</v>
@@ -14313,13 +14312,13 @@
     </row>
     <row r="144" spans="1:9" customFormat="1">
       <c r="A144" s="22" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="B144" s="23" t="s">
         <v>279</v>
       </c>
       <c r="C144" s="24" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="D144" s="45"/>
       <c r="E144" s="22" t="s">
@@ -14800,7 +14799,7 @@
         <v>31</v>
       </c>
       <c r="C163" s="24" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="D163" s="23"/>
       <c r="E163" s="22" t="s">
@@ -25595,7 +25594,7 @@
         <v>1138</v>
       </c>
       <c r="C592" s="24" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="D592" s="23"/>
       <c r="E592" s="22" t="s">
@@ -27771,7 +27770,7 @@
         <v>1333</v>
       </c>
       <c r="C679" s="24" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="D679" s="23"/>
       <c r="E679" s="22" t="s">
@@ -28240,13 +28239,13 @@
     </row>
     <row r="696" spans="1:9" customFormat="1" ht="86.4">
       <c r="A696" s="22" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="B696" s="23" t="s">
         <v>1339</v>
       </c>
       <c r="C696" s="24" t="s">
-        <v>1581</v>
+        <v>1591</v>
       </c>
       <c r="D696" s="30" t="s">
         <v>1579</v>
@@ -28275,7 +28274,7 @@
         <v>1333</v>
       </c>
       <c r="C697" s="24" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="D697" s="30" t="s">
         <v>1579</v>
@@ -28438,6 +28437,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -28445,11 +28449,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A578:B578 I620:I623 I679:I680 A294:B294 A514:C514 A116:C128 A131:C141 A517:C522 D525 A115:G115 A228:D228 A690:B691 I200 A688:C689 A692:C692 A240:C293 I41:I63 A310:I342 B169:D170 I169:I170 D295:H295 D116:H141 D577:D578 D524:E524 A344:I353 A152:I155 A151:H151 A157:I158 A156:H156 A160:I162 A159:H159 A229:H239 A526:D526 A529:D529 A142:H142 A343:H343 E656:I663 E655:H655 E665:I673 E664:H664 E675:I676 E674:H674 E677:H680 D517:H523 A515:D516 A196:H196 A354:H354 D240:I294 A20:H114 A164:I164 A163:H163 E624:I654 A296:I308 A309:H309 A355:I461 A579:D680 A702:D702 A171:I194 A693:D695 A685:D685 A682:I684 A681:H681 B165:I165 E166:H170 A198:H227 A464:I487 I497:I515 A488:D513 E488:H515 I539:I545 A532:D576 E526:H623 A696:C701 E685:H702 I547:I562 A143:I150">
@@ -30949,15 +30948,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -31006,6 +30996,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -31021,14 +31020,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31043,6 +31034,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>